<commit_message>
Fix: Improved error messages for emp/dict file loading issues
</commit_message>
<xml_diff>
--- a/data/dict_embbed.xlsx
+++ b/data/dict_embbed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projs\Peel Potato\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C2342F-BA52-45F2-8620-44604BB5F9CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3507FA-DC02-442C-8A9D-EA43BEFDA63D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
   <si>
     <t>old</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -354,6 +354,14 @@
   </si>
   <si>
     <t>直营管户连接年日均增量产能_年累计</t>
+  </si>
+  <si>
+    <t>当月晋升移交客户数(管户)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>晋升移交数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -688,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B97"/>
+  <dimension ref="A1:B98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="B98" sqref="A98:B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1201,9 +1209,17 @@
         <v>102</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>103</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>